<commit_message>
Add writing output files: salario, propina, viatico
</commit_message>
<xml_diff>
--- a/empleados_bac.xlsx
+++ b/empleados_bac.xlsx
@@ -109,7 +109,7 @@
     <t xml:space="preserve">JOSE MENENDEZ ARRIAZA</t>
   </si>
   <si>
-    <t xml:space="preserve">Jose Menendez</t>
+    <t xml:space="preserve">José Menéndez</t>
   </si>
   <si>
     <t xml:space="preserve">ANA DEL CARMEN ZOMETA </t>
@@ -311,7 +311,7 @@
       <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.91"/>

</xml_diff>

<commit_message>
Fix an issue with accents in vowels in empleados_bac.xlsx
</commit_message>
<xml_diff>
--- a/empleados_bac.xlsx
+++ b/empleados_bac.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">alias</t>
   </si>
   <si>
-    <t xml:space="preserve">SILVIA ELIZABETH AVENDA#O PINEDA  </t>
+    <t xml:space="preserve">SILVIA ELIZABETH AVENDANO PINEDA  </t>
   </si>
   <si>
     <t xml:space="preserve">Silvia</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">Juan</t>
   </si>
   <si>
-    <t xml:space="preserve">OSMIN ERNESTO RODRÍGUEZ</t>
+    <t xml:space="preserve">OSMIN ERNESTO RODRIGUEZ</t>
   </si>
   <si>
     <t xml:space="preserve">Ernesto</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">Doris</t>
   </si>
   <si>
-    <t xml:space="preserve">HANYI GRACIELA PEÑA ORELLANA</t>
+    <t xml:space="preserve">HANYI GRACIELA PENA ORELLANA</t>
   </si>
   <si>
     <t xml:space="preserve">Hanyi</t>
@@ -307,11 +307,11 @@
   </sheetPr>
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.91"/>

</xml_diff>

<commit_message>
Update test xlxs files to use ID (NIT and DUI)
</commit_message>
<xml_diff>
--- a/empleados_bac.xlsx
+++ b/empleados_bac.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t xml:space="preserve">alias</t>
   </si>
@@ -28,13 +28,16 @@
     <t xml:space="preserve">nombre</t>
   </si>
   <si>
-    <t xml:space="preserve">nit</t>
+    <t xml:space="preserve">id</t>
   </si>
   <si>
     <t xml:space="preserve">cuenta</t>
   </si>
   <si>
     <t xml:space="preserve">SILVIA ELIZABETH AVENDANO PINEDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRENDA GRISELDA ROMERO HERNANDEZ</t>
   </si>
   <si>
     <t xml:space="preserve">ANA MARISOL MENDOZA PINEDA     </t>
@@ -122,11 +125,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="00000000000000"/>
+    <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -148,21 +152,49 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FFD4D4D4"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD4D4D4"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD4D4D4"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD4D4D4"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -191,7 +223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -204,6 +236,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,6 +249,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFD4D4D4"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -221,13 +317,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.91"/>
@@ -264,18 +360,18 @@
         <v>118543040</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>5090808921119</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>118543057</v>
+      <c r="C3" s="3" t="n">
+        <v>55544433</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>122641731</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -286,10 +382,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>5081012951017</v>
+        <v>5090808921119</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>119693372</v>
+        <v>118543057</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,10 +396,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>5050502791023</v>
+        <v>5081012951017</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>118542950</v>
+        <v>119693372</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -314,10 +410,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>5051101781013</v>
+        <v>5050502791023</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>118542968</v>
+        <v>118542950</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -328,10 +424,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>5112912631010</v>
+        <v>5051101781013</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>118384072</v>
+        <v>118542968</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -342,10 +438,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>5051109851010</v>
+        <v>5112912631010</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>118557362</v>
+        <v>118384072</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,10 +452,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>5201811861026</v>
+        <v>5051109851010</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>118543032</v>
+        <v>118557362</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -370,10 +466,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>5051204931030</v>
+        <v>5201811861026</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>119693307</v>
+        <v>118543032</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,10 +480,10 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>5182502991018</v>
+        <v>5051204931030</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>119693380</v>
+        <v>119693307</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -398,10 +494,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>5111305791037</v>
+        <v>5182502991018</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>118558956</v>
+        <v>119693380</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -412,10 +508,10 @@
         <v>15</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>5051708951015</v>
+        <v>5111305791037</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>118543065</v>
+        <v>118558956</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,10 +522,10 @@
         <v>16</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>5111010470024</v>
+        <v>5051708951015</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>119693331</v>
+        <v>118543065</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,10 +536,10 @@
         <v>17</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>5111501510010</v>
+        <v>5111010470024</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>119693349</v>
+        <v>119693331</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,10 +550,10 @@
         <v>18</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>5110903001052</v>
+        <v>5111501510010</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>119693323</v>
+        <v>119693349</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,10 +564,10 @@
         <v>19</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>5081604961031</v>
+        <v>5110903001052</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>120212998</v>
+        <v>119693323</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,10 +578,10 @@
         <v>20</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>5182108971010</v>
+        <v>5081604961031</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>119693364</v>
+        <v>120212998</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,10 +592,10 @@
         <v>21</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>5050311961026</v>
+        <v>5182108971010</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>120232830</v>
+        <v>119693364</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,10 +606,10 @@
         <v>22</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>5080709981015</v>
+        <v>5050311961026</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>119942969</v>
+        <v>120232830</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -524,10 +620,10 @@
         <v>23</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>6142310011500</v>
+        <v>5080709981015</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>119938462</v>
+        <v>119942969</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -538,10 +634,10 @@
         <v>24</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>5112211961148</v>
+        <v>6142310011500</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>119938470</v>
+        <v>119938462</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,10 +648,10 @@
         <v>25</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>5051904981011</v>
+        <v>5112211961148</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>119693299</v>
+        <v>119938470</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -566,10 +662,10 @@
         <v>26</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>5051208011024</v>
+        <v>5051904981011</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>119693356</v>
+        <v>119693299</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,10 +676,10 @@
         <v>27</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>5182708971013</v>
+        <v>5051208011024</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>119693315</v>
+        <v>119693356</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,10 +690,10 @@
         <v>28</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>5080705001016</v>
+        <v>5182708971013</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>119938488</v>
+        <v>119693315</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,10 +704,10 @@
         <v>29</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>5051702981028</v>
+        <v>5080705001016</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>119943058</v>
+        <v>119938488</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,10 +718,10 @@
         <v>30</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>5082509881019</v>
+        <v>5051702981028</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>119938454</v>
+        <v>119943058</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,9 +732,23 @@
         <v>31</v>
       </c>
       <c r="C29" s="2" t="n">
+        <v>5082509881019</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>119938454</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="2" t="n">
         <v>5081803921014</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D30" s="1" t="n">
         <v>118065762</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add DUI as ID in integration test files
</commit_message>
<xml_diff>
--- a/empleados_bac.xlsx
+++ b/empleados_bac.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t xml:space="preserve">alias</t>
   </si>
@@ -37,7 +37,22 @@
     <t xml:space="preserve">SILVIA ELIZABETH AVENDANO PINEDA</t>
   </si>
   <si>
+    <t xml:space="preserve">BRENDA ROMERO HERNANDEZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">BRENDA GRISELDA ROMERO HERNANDEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRENDA ROMERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">054354354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRISELDA HERNANDEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">012345678 </t>
   </si>
   <si>
     <t xml:space="preserve">ANA MARISOL MENDOZA PINEDA     </t>
@@ -317,13 +332,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.91"/>
@@ -365,7 +380,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>55544433</v>
@@ -374,381 +389,409 @@
         <v>122641731</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>122641732</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>5090808921119</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>118543057</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>5081012951017</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>119693372</v>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>122641733</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>5050502791023</v>
+        <v>5090808921119</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>118542950</v>
+        <v>118543057</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>5051101781013</v>
+        <v>5081012951017</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>118542968</v>
+        <v>119693372</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>5112912631010</v>
+        <v>5050502791023</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>118384072</v>
+        <v>118542950</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>5051109851010</v>
+        <v>5051101781013</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>118557362</v>
+        <v>118542968</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>5201811861026</v>
+        <v>5112912631010</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>118543032</v>
+        <v>118384072</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>5051204931030</v>
+        <v>5051109851010</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>119693307</v>
+        <v>118557362</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>5182502991018</v>
+        <v>5201811861026</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>119693380</v>
+        <v>118543032</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>5111305791037</v>
+        <v>5051204931030</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>118558956</v>
+        <v>119693307</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>5051708951015</v>
+        <v>5182502991018</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>118543065</v>
+        <v>119693380</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>5111010470024</v>
+        <v>5111305791037</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>119693331</v>
+        <v>118558956</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>5111501510010</v>
+        <v>5051708951015</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>119693349</v>
+        <v>118543065</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>5110903001052</v>
+        <v>5111010470024</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>119693323</v>
+        <v>119693331</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>5081604961031</v>
+        <v>5111501510010</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>120212998</v>
+        <v>119693349</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>5182108971010</v>
+        <v>5110903001052</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>119693364</v>
+        <v>119693323</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>5050311961026</v>
+        <v>5081604961031</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>120232830</v>
+        <v>120212998</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>5080709981015</v>
+        <v>5182108971010</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>119942969</v>
+        <v>119693364</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>6142310011500</v>
+        <v>5050311961026</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>119938462</v>
+        <v>120232830</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>5112211961148</v>
+        <v>5080709981015</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>119938470</v>
+        <v>119942969</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>5051904981011</v>
+        <v>6142310011500</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>119693299</v>
+        <v>119938462</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>5051208011024</v>
+        <v>5112211961148</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>119693356</v>
+        <v>119938470</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>5182708971013</v>
+        <v>5051904981011</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>119693315</v>
+        <v>119693299</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>5080705001016</v>
+        <v>5051208011024</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>119938488</v>
+        <v>119693356</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>5051702981028</v>
+        <v>5182708971013</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>119943058</v>
+        <v>119693315</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>5082509881019</v>
+        <v>5080705001016</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>119938454</v>
+        <v>119938488</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C30" s="2" t="n">
+        <v>5051702981028</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>119943058</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>5082509881019</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>119938454</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="2" t="n">
         <v>5081803921014</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D32" s="1" t="n">
         <v>118065762</v>
       </c>
     </row>

</xml_diff>